<commit_message>
Report5.blade, report5export, adminutilityController, cerpen
</commit_message>
<xml_diff>
--- a/supportfile/todolist.xlsx
+++ b/supportfile/todolist.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\xampp\htdocs\sentul-apps\supportfile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
@@ -16,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
-  <si>
-    <t>Update 10/04/2019</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Menu</t>
   </si>
@@ -30,71 +32,20 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
     <t>Keterangan</t>
   </si>
   <si>
-    <t>MasterApp</t>
-  </si>
-  <si>
-    <t>Penambahan field Singkatan di table company</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Jenis Update</t>
   </si>
-  <si>
-    <t>Penambahan field input baru</t>
-  </si>
-  <si>
-    <t>Penambahan Menu Baru ( Add, Edit, Update)</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (brand) di masterapps database</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Produk</t>
-  </si>
-  <si>
-    <t>Mesin Filling</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (mesin_filling) di masterapps database</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (produk) di masterapps database</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (plan) di masterapps database</t>
-  </si>
-  <si>
-    <t>Kelompok Mesin Filling</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (mesin_filling_head dan mesin_filling_detail) di masterapps database</t>
-  </si>
-  <si>
-    <t>Jenis Produk</t>
-  </si>
-  <si>
-    <t>Penambahan table baru (jenis_produk) di masterapps database</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,9 +91,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -152,12 +100,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,9 +195,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,6 +230,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,14 +406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -462,152 +423,37 @@
     <col min="6" max="6" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="23.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -619,24 +465,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>